<commit_message>
changed them excel files
</commit_message>
<xml_diff>
--- a/Extraction Description.xlsx
+++ b/Extraction Description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minsik/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D289CDBB-3791-AA45-9A81-72AD8A40DA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{00675EB4-A62A-FE49-BDF5-3EE044825D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40680" yWindow="4800" windowWidth="27640" windowHeight="16800" xr2:uid="{8FA1A399-579C-054D-B807-8F20E9FA9D03}"/>
+    <workbookView xWindow="36120" yWindow="1040" windowWidth="27640" windowHeight="16800" xr2:uid="{89054DD3-541D-2F43-91F8-5BD17A2C6CD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -113,6 +113,10 @@
     <t>OS</t>
   </si>
   <si>
+    <t>HF,HFES,ERGO IN DE</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Final</t>
   </si>
   <si>
@@ -132,9 +136,6 @@
   </si>
   <si>
     <t>T&amp;F</t>
-  </si>
-  <si>
-    <t>HF,HFES,ERGO IN DE</t>
   </si>
 </sst>
 </file>
@@ -581,11 +582,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5469098-B8AA-0745-B780-A80C263A8627}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E2588FF-AA31-A545-883B-61C6B9809A36}">
   <dimension ref="A2:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1006,7 +1007,7 @@
         <v>4</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -1035,7 +1036,7 @@
         <v>10</v>
       </c>
       <c r="O18" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
@@ -1062,7 +1063,7 @@
         <v>7</v>
       </c>
       <c r="O19" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P19" s="11" t="s">
         <v>21</v>
@@ -1138,7 +1139,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1146,7 +1147,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
@@ -1156,7 +1157,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1274,7 +1275,7 @@
         <v>0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1282,7 +1283,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>

</xml_diff>